<commit_message>
updated cart features and buyer pages
</commit_message>
<xml_diff>
--- a/public/exel/test.xlsx
+++ b/public/exel/test.xlsx
@@ -16,12 +16,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>products/</t>
   </si>
   <si>
-    <t>a.jpg</t>
+    <t>Samsung Galaxy S23</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>Smartphone flagship dengan layar Dynamic AMOLED 6.1 inci, prosesor Snapdragon 8 Gen 2, dan kamera utama 50 MP.</t>
+  </si>
+  <si>
+    <t>Apple MacBook Air M2</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Laptop ringan dan bertenaga dengan chip Apple M2, layar Retina 13.6 inci, dan daya tahan baterai hingga 18 jam.</t>
+  </si>
+  <si>
+    <t>Sony WH-1000XM5</t>
+  </si>
+  <si>
+    <t>Headphone</t>
+  </si>
+  <si>
+    <t>Headphone noise-cancelling premium dengan driver 30 mm, konektivitas Bluetooth 5.2, dan masa pakai baterai hingga 30 jam.</t>
+  </si>
+  <si>
+    <t>LG OLED C3</t>
+  </si>
+  <si>
+    <t>Televisi</t>
+  </si>
+  <si>
+    <t>Televisi OLED 55 inci dengan resolusi 4K UHD, dukungan HDR10, Dolby Vision, dan sistem operasi WebOS.</t>
+  </si>
+  <si>
+    <t>Dyson V15 Detect</t>
+  </si>
+  <si>
+    <t>Vacuum Cleaner</t>
+  </si>
+  <si>
+    <t>Vacuum cleaner nirkabel dengan teknologi laser untuk mendeteksi debu mikro dan daya hisap kuat.</t>
+  </si>
+  <si>
+    <t>.jpg</t>
+  </si>
+  <si>
+    <t>Xiaomi Redmi Note 12 Pro</t>
+  </si>
+  <si>
+    <t>Smartphone mid-range dengan layar AMOLED 6.67 inci, kamera utama 108 MP, dan baterai 5000 mAh.</t>
+  </si>
+  <si>
+    <t>ASUS ROG Zephyrus G14</t>
+  </si>
+  <si>
+    <t>Laptop gaming dengan prosesor AMD Ryzen 9, GPU RTX 4060, dan layar 14 inci QHD 120Hz.</t>
+  </si>
+  <si>
+    <t>JBL Charge 5</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>Speaker portabel dengan suara bass kuat, tahan air, dan baterai tahan hingga 20 jam.</t>
+  </si>
+  <si>
+    <t>Canon EOS R50</t>
+  </si>
+  <si>
+    <t>Kamera</t>
+  </si>
+  <si>
+    <t>Kamera mirrorless dengan sensor APS-C 24.2 MP, ideal untuk fotografi dan vlogging.</t>
+  </si>
+  <si>
+    <t>Samsung Smart Monitor M8</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Monitor 32 inci dengan resolusi 4K UHD, fitur Smart Hub, dan dukungan AirPlay 2.</t>
+  </si>
+  <si>
+    <t>Dyson Pure Cool TP07</t>
+  </si>
+  <si>
+    <t>Air Purifier</t>
+  </si>
+  <si>
+    <t>Air purifier sekaligus kipas angin dengan teknologi HEPA dan pengendalian via aplikasi.</t>
+  </si>
+  <si>
+    <t>Logitech MX Master 3S</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Mouse wireless ergonomis dengan sensor 8.000 DPI dan baterai tahan hingga 70 hari.</t>
+  </si>
+  <si>
+    <t>Panasonic Lumix GH6</t>
+  </si>
+  <si>
+    <t>Kamera mirrorless dengan sensor Micro Four Thirds 25.2 MP, cocok untuk videografi profesional.</t>
+  </si>
+  <si>
+    <t>PlayStation 5</t>
+  </si>
+  <si>
+    <t>Konsol</t>
+  </si>
+  <si>
+    <t>Konsol gaming generasi terbaru dengan prosesor AMD Ryzen dan dukungan game hingga 4K 120fps.</t>
+  </si>
+  <si>
+    <t>Midea MFM-20CRN1</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Air conditioner 1 PK dengan fitur hemat energi dan pendinginan cepat.</t>
   </si>
 </sst>
 </file>
@@ -57,8 +183,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,38 +481,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="28.5546875" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2">
+        <v>13999000</v>
+      </c>
+      <c r="E1" s="1">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>16999000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>4999000</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
+        <v>24999000</v>
+      </c>
+      <c r="E4" s="1">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>10999000</v>
+      </c>
+      <c r="E5" s="1">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>5</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4499000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>23999000</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2499000</v>
+      </c>
+      <c r="E8" s="1">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>8</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2">
+        <v>12999000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>9</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8499000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>10</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2">
+        <v>12499000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>11</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1599000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>12</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2">
+        <v>34999000</v>
+      </c>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9999000</v>
+      </c>
+      <c r="E14" s="1">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>14</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="2">
+        <v>3999000</v>
+      </c>
+      <c r="E15" s="1">
+        <v>25</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>15</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>